<commit_message>
add memorizer sft baselines
</commit_message>
<xml_diff>
--- a/exp_output/Llama-3.2-1B-eos-sft_sft-baseline_input=2hop_lr=1e-05_epoch=1.0_tune_num_epoch/individual_results/2hop__460946_294723_eval_results.xlsx
+++ b/exp_output/Llama-3.2-1B-eos-sft_sft-baseline_input=2hop_lr=1e-05_epoch=1.0_tune_num_epoch/individual_results/2hop__460946_294723_eval_results.xlsx
@@ -548,7 +548,8 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Who is the performer associated with Green?</t>
+          <t>who is the performer associated with green?
+?</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -561,7 +562,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Jethro Tull</t>
+          <t>JIMMY SAVILE</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -592,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>0.3333333432674408</v>
+        <v>0.3076923191547394</v>
       </c>
     </row>
     <row r="3">
@@ -618,7 +619,8 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Who is the spouse of Steve Hillage?</t>
+          <t>who is the spouse of steve hillage?
+?</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -631,26 +633,26 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Miquette</t>
+          <t>MARY ANNE HOBBS</t>
         </is>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>

</xml_diff>